<commit_message>
Updated stream graph almost complete
</commit_message>
<xml_diff>
--- a/Visualisation 2/DataProcessing/EnergyGen.xlsx
+++ b/Visualisation 2/DataProcessing/EnergyGen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THhum\Documents\Uni\2024 Sem 2\FIT3179\FIT3179\Visualisation 2\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D48FE7D-EA77-409C-9F16-A472EA642174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DC8A0C-D513-4424-8753-AAF89EB7877B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-1330" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,43 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
-    <t xml:space="preserve">  Black coal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Brown coal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Natural gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Oil products</t>
-  </si>
-  <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Bagasse, wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Biogas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Hydro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Large-scale solar PV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Small-scale solar PV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Geothermal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Other non-renewable</t>
   </si>
   <si>
     <t>Fuel Type</t>
@@ -85,18 +49,55 @@
   <si>
     <t>Renewable</t>
   </si>
+  <si>
+    <t>Black coal</t>
+  </si>
+  <si>
+    <t>Brown coal</t>
+  </si>
+  <si>
+    <t>Natural gas</t>
+  </si>
+  <si>
+    <t>Oil products</t>
+  </si>
+  <si>
+    <t>Other non-renewable</t>
+  </si>
+  <si>
+    <t>Bagasse, wood</t>
+  </si>
+  <si>
+    <t>Biogas</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Hydro</t>
+  </si>
+  <si>
+    <t>Large-scale solar PV</t>
+  </si>
+  <si>
+    <t>Small-scale solar PV</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +259,32 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -533,7 +560,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="401">
+  <cellStyleXfs count="408">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
@@ -997,11 +1024,27 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="406" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="407" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="401">
+  <cellStyles count="408">
     <cellStyle name="20% - Accent1 2" xfId="3" xr:uid="{E3184A2C-0CDF-4343-A6D2-F045F321BC0A}"/>
     <cellStyle name="20% - Accent2 2" xfId="4" xr:uid="{231785E3-409E-45A7-867D-7C9FCBFDB209}"/>
     <cellStyle name="20% - Accent3 2" xfId="5" xr:uid="{D29B77EF-9567-4429-8D6C-09CE9BFDC4F4}"/>
@@ -1034,6 +1077,7 @@
     <cellStyle name="Comma 2 2" xfId="32" xr:uid="{7F315EA1-5177-4B2B-9689-4F4E5726D1B2}"/>
     <cellStyle name="Comma 2 2 2" xfId="33" xr:uid="{EFA33D2C-26D3-4290-9F4C-AB63C0C06698}"/>
     <cellStyle name="Comma 2 3" xfId="34" xr:uid="{25E76F90-BFE1-4334-9EE5-0A67450BF811}"/>
+    <cellStyle name="Comma 2 4" xfId="402" xr:uid="{6070D9F2-53F8-4B7A-AEE3-2551D8518A2F}"/>
     <cellStyle name="Comma 3" xfId="35" xr:uid="{E83327E0-84A4-42CD-865A-9B137A77D86E}"/>
     <cellStyle name="Comma 3 2" xfId="36" xr:uid="{AB9483F9-348B-41D6-990C-D4603BAFE194}"/>
     <cellStyle name="Comma 4" xfId="37" xr:uid="{EED7AB55-1739-42A8-A96C-64CE0A672A1A}"/>
@@ -1071,6 +1115,7 @@
     <cellStyle name="Cover 4 3 3" xfId="68" xr:uid="{F268E605-94B6-49DD-9AC3-21037FCA2354}"/>
     <cellStyle name="Cover 4 4" xfId="69" xr:uid="{9197DB29-6848-4637-8336-1CE271B31822}"/>
     <cellStyle name="Explanatory Text 2" xfId="70" xr:uid="{5BC20BAF-C003-423D-9D22-E1A36B3A6E67}"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" xr:uid="{BAC16538-64F4-41DC-AF8A-BA76B576D13F}"/>
     <cellStyle name="Good 2" xfId="71" xr:uid="{E790FE90-9999-4314-B3D6-BB2B444A4CC2}"/>
     <cellStyle name="Heading 1 2" xfId="72" xr:uid="{5FA4BB29-E9E7-4564-9991-8F0B746467BC}"/>
     <cellStyle name="Heading 2 2" xfId="73" xr:uid="{9187DCE3-1C75-448F-89F4-FB771635B7F1}"/>
@@ -1188,14 +1233,18 @@
     <cellStyle name="Normal 156 2 2" xfId="182" xr:uid="{7BB1A0C9-5E13-45CF-B6F2-F28DCCBA15CB}"/>
     <cellStyle name="Normal 156 3" xfId="183" xr:uid="{7C734956-5ED5-49C9-A764-7A5DF2D81A2F}"/>
     <cellStyle name="Normal 156_pivot" xfId="184" xr:uid="{3FCAEFCF-A41C-44D5-A714-AC215DB1EF3F}"/>
+    <cellStyle name="Normal 16" xfId="407" xr:uid="{68C39C7B-3145-47C3-9460-1AD416BBAD35}"/>
     <cellStyle name="Normal 16 2" xfId="185" xr:uid="{AC80F847-7B53-4881-9087-2143591645BD}"/>
+    <cellStyle name="Normal 17" xfId="406" xr:uid="{63817933-5AC6-45C1-ADCA-8ADBB8514A52}"/>
     <cellStyle name="Normal 17 2" xfId="186" xr:uid="{FA1A0B4D-1B81-47CF-B6E2-948C2388A731}"/>
     <cellStyle name="Normal 18 2" xfId="187" xr:uid="{0FCD67D5-1120-4FAC-B814-9D21019ABFA5}"/>
     <cellStyle name="Normal 19 2" xfId="188" xr:uid="{4DD5D71C-DC74-42A1-BD19-01D4705EB628}"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{66315A38-3E2D-4A89-9C09-2A4A0B642EFD}"/>
     <cellStyle name="Normal 2 10" xfId="189" xr:uid="{4B567F62-5F94-47B1-B5B2-7A1474CF879B}"/>
+    <cellStyle name="Normal 2 11" xfId="404" xr:uid="{39DA932E-7D86-4A31-A597-D8A9A1414A75}"/>
     <cellStyle name="Normal 2 12" xfId="399" xr:uid="{76B7707D-9211-4CD2-9FD1-A8BDD1CF958D}"/>
     <cellStyle name="Normal 2 2" xfId="190" xr:uid="{CEE464B3-1A43-46B2-B347-B50DDFBCECB0}"/>
+    <cellStyle name="Normal 2 2 2" xfId="403" xr:uid="{CB8E0C23-E534-483D-8794-303AE3EA8267}"/>
     <cellStyle name="Normal 2 3" xfId="191" xr:uid="{F93F4F20-41C6-46F4-ABFD-B8156290E87D}"/>
     <cellStyle name="Normal 2 4" xfId="192" xr:uid="{83233156-B5F5-4DC1-8088-A5A9E464B3C6}"/>
     <cellStyle name="Normal 2 5" xfId="193" xr:uid="{FB56DC32-206C-4B80-AC58-928D2E1BFE55}"/>
@@ -1381,6 +1430,7 @@
     <cellStyle name="Percent 2 2" xfId="373" xr:uid="{C22A690B-3DE9-4375-9170-DE7CC736CB07}"/>
     <cellStyle name="Percent 2 2 2" xfId="374" xr:uid="{58C8CFAA-3A4B-43B0-8431-470BCDFE94BD}"/>
     <cellStyle name="Percent 2 3" xfId="375" xr:uid="{2EA280B0-3FFF-4EAE-A382-11F6256F0FAB}"/>
+    <cellStyle name="Percent 2 4" xfId="401" xr:uid="{352BCA97-F2BA-48BA-B8E9-612562EF1D73}"/>
     <cellStyle name="Percent 3" xfId="376" xr:uid="{62E36E5D-B142-4CAB-80AF-B70CEEAFB7CB}"/>
     <cellStyle name="Percent 4" xfId="377" xr:uid="{A712B841-1B44-478C-B6E6-8A448E4471DF}"/>
     <cellStyle name="Percent 4 2" xfId="378" xr:uid="{FE4E8F02-2914-46D9-849A-B32A35F66679}"/>
@@ -1680,23 +1730,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AD25" sqref="AD25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="6" max="34" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1">
         <v>1989</v>
@@ -1829,13 +1880,16 @@
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
+      <c r="AJ1">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>87573</v>
@@ -1936,13 +1990,16 @@
       <c r="AI2">
         <v>101076.158</v>
       </c>
+      <c r="AJ2" s="1">
+        <v>96173.858193717693</v>
+      </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>33594</v>
@@ -2043,13 +2100,16 @@
       <c r="AI3">
         <v>32515.635999999999</v>
       </c>
+      <c r="AJ3" s="1">
+        <v>31459.125523381801</v>
+      </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
       <c r="C4">
         <v>14359</v>
@@ -2150,13 +2210,16 @@
       <c r="AI4">
         <v>49280.224999999999</v>
       </c>
+      <c r="AJ4" s="1">
+        <v>48865.237380704799</v>
+      </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>3552</v>
@@ -2257,13 +2320,16 @@
       <c r="AI5">
         <v>4663.9960000000001</v>
       </c>
+      <c r="AJ5" s="1">
+        <v>4864.3971483286441</v>
+      </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2364,13 +2430,16 @@
       <c r="AI6">
         <v>0</v>
       </c>
+      <c r="AJ6" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>750</v>
@@ -2471,13 +2540,16 @@
       <c r="AI7">
         <v>1817.451</v>
       </c>
+      <c r="AJ7" s="2">
+        <v>1687.7196683510799</v>
+      </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:36">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -2578,13 +2650,16 @@
       <c r="AI8">
         <v>1372.806</v>
       </c>
+      <c r="AJ8" s="2">
+        <v>1405.0737606722</v>
+      </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2685,13 +2760,16 @@
       <c r="AI9">
         <v>29107.793000000001</v>
       </c>
+      <c r="AJ9" s="2">
+        <v>31384.873888888898</v>
+      </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:36">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>14880</v>
@@ -2792,13 +2870,16 @@
       <c r="AI10">
         <v>17010.891</v>
       </c>
+      <c r="AJ10" s="2">
+        <v>16666.054444444399</v>
+      </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:36">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2899,13 +2980,16 @@
       <c r="AI11">
         <v>12569.175999999999</v>
       </c>
+      <c r="AJ11" s="2">
+        <v>16059.8195145678</v>
+      </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:36">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3006,13 +3090,16 @@
       <c r="AI12">
         <v>22117.45</v>
       </c>
+      <c r="AJ12" s="2">
+        <v>25908.682159</v>
+      </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -3111,6 +3198,9 @@
         <v>0</v>
       </c>
       <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>